<commit_message>
More work on plots and tables
</commit_message>
<xml_diff>
--- a/RealWorldStudy/realWorldTable.xlsx
+++ b/RealWorldStudy/realWorldTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/schuemie/git/ImprovingEvidenceSynthesis/RealWorldStudy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{4BBFB8EE-C654-EE4F-860C-02FB9DB285A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F9220EF-4106-0048-B1BD-4006BAC27AD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30240" yWindow="-9160" windowWidth="51200" windowHeight="28800" xr2:uid="{6648D796-5CD5-724F-8970-1E2F32A0FFBF}"/>
   </bookViews>
@@ -52,9 +52,6 @@
     <t>1.72 (0.66-3.68)</t>
   </si>
   <si>
-    <t>Normal fixed-effects</t>
-  </si>
-  <si>
     <t>1.51 (0.85-2.66)</t>
   </si>
   <si>
@@ -64,58 +61,61 @@
     <t>Pooled fixed-effects</t>
   </si>
   <si>
-    <t>Custom random-effects</t>
-  </si>
-  <si>
     <t>1.27 (0.62-2.59)</t>
   </si>
   <si>
     <t>1.53 (0.56-3.87)</t>
   </si>
   <si>
-    <t>Grid random-effects</t>
-  </si>
-  <si>
     <t>1.27 (0.61-2.60)</t>
   </si>
   <si>
     <t>1.53 (0.56-4.00)</t>
   </si>
   <si>
-    <t>Hermite interpolation random-effects</t>
-  </si>
-  <si>
     <t>1.28 (0.62-2.66)</t>
   </si>
   <si>
     <t>1.49 (0.55-3.70)</t>
   </si>
   <si>
-    <t>Normal random-effects</t>
-  </si>
-  <si>
     <t>1.49 (0.74-3.00)</t>
   </si>
   <si>
     <t>1.89 (0.70-5.09)</t>
   </si>
   <si>
-    <t>Pooled random-effects</t>
-  </si>
-  <si>
     <t>1.27 (0.62-2.63)</t>
   </si>
   <si>
     <t>1.51 (0.59-3.90)</t>
   </si>
   <si>
-    <t>Normal traditional random-effects</t>
-  </si>
-  <si>
     <t>1.50 (0.78-2.86)</t>
   </si>
   <si>
     <t>Method</t>
+  </si>
+  <si>
+    <t>Traditional random-effects</t>
+  </si>
+  <si>
+    <t>Traditional fixed-effects</t>
+  </si>
+  <si>
+    <t>Custom Bayesian random-effects</t>
+  </si>
+  <si>
+    <t>Pooled Bayesian random-effects</t>
+  </si>
+  <si>
+    <t>Grid Bayesian random-effects</t>
+  </si>
+  <si>
+    <t>Hermite interpolation Bayesian random-effects</t>
+  </si>
+  <si>
+    <t>Normal Bayesian random-effects</t>
   </si>
 </sst>
 </file>
@@ -635,12 +635,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1019,18 +1020,18 @@
   <dimension ref="A2:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>0</v>
@@ -1041,7 +1042,7 @@
     </row>
     <row r="3" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
@@ -1052,112 +1053,112 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" t="s">
-        <v>16</v>
+      <c r="A9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>